<commit_message>
Split Pelagic groups from benthic groups to create new file.  Fixed ecosystem names to make them consistent with those used in the dataset, which differ from the report.
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\MarineCoastal-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Marine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97C3E19-FB9E-4B4E-9A46-336E83AB1886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FCD06E-BC4B-4E26-8DA2-B304487E304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="160">
   <si>
     <t>Realm</t>
   </si>
@@ -447,18 +447,6 @@
     <t>get:groups/M1.5</t>
   </si>
   <si>
-    <t>get:groups/M2.1</t>
-  </si>
-  <si>
-    <t>get:groups/M2.2</t>
-  </si>
-  <si>
-    <t>get:groups/M2.3</t>
-  </si>
-  <si>
-    <t>get:groups/M2.4</t>
-  </si>
-  <si>
     <t>creator_id: https://orcid.org/0000-0002-3884-3420</t>
   </si>
   <si>
@@ -492,33 +480,18 @@
     <t>nesp:Shelf-unvegetated-sediments</t>
   </si>
   <si>
-    <t>nesp:Upper-slope-sediments</t>
-  </si>
-  <si>
     <t>nesp:Mid-slope-sediments</t>
   </si>
   <si>
-    <t>nesp:Lower-slope-reef-&amp;-sediments</t>
-  </si>
-  <si>
-    <t>nesp:Abyss-reefs-&amp;-sediments</t>
-  </si>
-  <si>
     <t>nesp:Seamount-sediments</t>
   </si>
   <si>
     <t>nesp:Seamount-reefs</t>
   </si>
   <si>
-    <t>nesp:Shelf-incising-canyons</t>
-  </si>
-  <si>
     <t>nesp:Shelf-vegetated-sediments</t>
   </si>
   <si>
-    <t>nesp:Oceanic-coral-reefs</t>
-  </si>
-  <si>
     <t>nesp:Oceanic-shallow-coral-reefs</t>
   </si>
   <si>
@@ -534,28 +507,52 @@
     <t>nesp:Oceanic-mesophotic-coral-reefs</t>
   </si>
   <si>
-    <t>nesp:Rariphotic-shelf-reefs</t>
-  </si>
-  <si>
     <t>nesp:Upper-slope-reefs</t>
   </si>
   <si>
-    <t>nesp:Mid-slope-reefs</t>
-  </si>
-  <si>
-    <t>nesp:On-shelf-(neritic)-epinesp</t>
-  </si>
-  <si>
-    <t>nesp:Off-shelf-(oceanic)-epinesp</t>
-  </si>
-  <si>
-    <t>nesp:Mesonesp</t>
-  </si>
-  <si>
-    <t>nesp:Bathynesp-&amp;-Abyssonesp</t>
-  </si>
-  <si>
     <t>author_label</t>
+  </si>
+  <si>
+    <t>Upper slope unvegetated sediments</t>
+  </si>
+  <si>
+    <t>nesp:Upper-slope-unvegetated-sediments</t>
+  </si>
+  <si>
+    <t>Mid slope sediments</t>
+  </si>
+  <si>
+    <t>Lower slope reef and soft sediments</t>
+  </si>
+  <si>
+    <t>Abyssal reef and sediments</t>
+  </si>
+  <si>
+    <t>nesp:Lower-slope-reef-and-soft-sediments</t>
+  </si>
+  <si>
+    <t>nesp:Abyssal-reef-and-sediments</t>
+  </si>
+  <si>
+    <t>Shelf incised canyons</t>
+  </si>
+  <si>
+    <t>nesp:Shelf-incised-canyons</t>
+  </si>
+  <si>
+    <t>Mid slope reef</t>
+  </si>
+  <si>
+    <t>nesp:Mid-slope-reef</t>
+  </si>
+  <si>
+    <t>Rariophotic shelf reefs</t>
+  </si>
+  <si>
+    <t>nesp:Rariophotic-shelf-reefs</t>
+  </si>
+  <si>
+    <t>Shallow coral reefs</t>
   </si>
 </sst>
 </file>
@@ -625,7 +622,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +641,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -657,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -676,6 +685,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,7 +1018,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD30"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1326,7 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1341,7 +1352,7 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1419,7 +1430,7 @@
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1471,7 +1482,7 @@
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1709,7 +1720,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,52 +2320,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2364,16 +2375,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
@@ -2412,7 +2423,7 @@
         <v>90</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>91</v>
@@ -2436,9 +2447,9 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -2477,9 +2488,9 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
@@ -2518,9 +2529,9 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -2559,9 +2570,9 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
@@ -2600,10 +2611,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
+        <v>147</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>95</v>
@@ -2641,10 +2652,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
+        <v>135</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="C7" t="s">
         <v>95</v>
@@ -2682,10 +2693,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
+        <v>151</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>95</v>
@@ -2723,10 +2734,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+        <v>152</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="C9" t="s">
         <v>98</v>
@@ -2764,9 +2775,9 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
@@ -2805,9 +2816,9 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C11" t="s">
@@ -2846,10 +2857,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
+        <v>154</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="C12" t="s">
         <v>98</v>
@@ -2887,9 +2898,9 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
@@ -2928,10 +2939,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
+        <v>143</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>95</v>
@@ -2969,10 +2980,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
+        <v>139</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="C15" t="s">
         <v>95</v>
@@ -3010,9 +3021,9 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C16" t="s">
@@ -3051,9 +3062,9 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
@@ -3092,9 +3103,9 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C18" t="s">
@@ -3133,10 +3144,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
+        <v>141</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>95</v>
@@ -3174,9 +3185,9 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
@@ -3215,9 +3226,9 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C21" t="s">
@@ -3256,10 +3267,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
+        <v>158</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="C22" t="s">
         <v>95</v>
@@ -3297,9 +3308,9 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C23" t="s">
@@ -3338,10 +3349,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>154</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
+        <v>156</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="C24" t="s">
         <v>95</v>
@@ -3376,255 +3387,6 @@
       <c r="N24" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K25" t="s">
-        <v>108</v>
-      </c>
-      <c r="L25" t="s">
-        <v>103</v>
-      </c>
-      <c r="M25" t="s">
-        <v>109</v>
-      </c>
-      <c r="N25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I26" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K26" t="s">
-        <v>108</v>
-      </c>
-      <c r="L26" t="s">
-        <v>103</v>
-      </c>
-      <c r="M26" t="s">
-        <v>109</v>
-      </c>
-      <c r="N26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>157</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K27" t="s">
-        <v>108</v>
-      </c>
-      <c r="L27" t="s">
-        <v>103</v>
-      </c>
-      <c r="M27" t="s">
-        <v>109</v>
-      </c>
-      <c r="N27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>158</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" t="s">
-        <v>94</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H28" t="s">
-        <v>106</v>
-      </c>
-      <c r="I28" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K28" t="s">
-        <v>108</v>
-      </c>
-      <c r="L28" t="s">
-        <v>103</v>
-      </c>
-      <c r="M28" t="s">
-        <v>109</v>
-      </c>
-      <c r="N28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" t="s">
-        <v>94</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H29" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K29" t="s">
-        <v>108</v>
-      </c>
-      <c r="L29" t="s">
-        <v>103</v>
-      </c>
-      <c r="M29" t="s">
-        <v>109</v>
-      </c>
-      <c r="N29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>159</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" t="s">
-        <v>94</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H30" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="9">
-        <v>45292</v>
-      </c>
-      <c r="K30" t="s">
-        <v>108</v>
-      </c>
-      <c r="L30" t="s">
-        <v>103</v>
-      </c>
-      <c r="M30" t="s">
-        <v>109</v>
-      </c>
-      <c r="N30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G31" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3633,65 +3395,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -3967,7 +3670,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
@@ -3984,23 +3687,66 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4019,7 +3765,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4028,4 +3774,20 @@
     <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to Marine crosswalk - adding two categories in attribute table to crosswalk
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Marine-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jor069_csiro_au/Documents/NEAP/Crosswalks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FCD06E-BC4B-4E26-8DA2-B304487E304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31CCD48D-FB0C-4743-8FA7-805ABE564F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk_V1" sheetId="1" r:id="rId1"/>
     <sheet name="Crosswalk_V2" sheetId="3" r:id="rId2"/>
     <sheet name="header" sheetId="5" r:id="rId3"/>
     <sheet name="SSSOM" sheetId="4" r:id="rId4"/>
+    <sheet name="CHANGE_LOG" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="174">
   <si>
     <t>Realm</t>
   </si>
@@ -554,12 +555,54 @@
   <si>
     <t>Shallow coral reefs</t>
   </si>
+  <si>
+    <t>nesp:Islands-including-cays-and-islets</t>
+  </si>
+  <si>
+    <t>Islands (including cays and islets)</t>
+  </si>
+  <si>
+    <t>owl:Nothing</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>orcid:0000-0002-4048-6792</t>
+  </si>
+  <si>
+    <t>Rebecca Jordan</t>
+  </si>
+  <si>
+    <t>status:draft</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>Islands (incluidng cays and islets)' and 'Mesophotic coral reefs' added to crosswalk to match attribute table of marine data</t>
+  </si>
+  <si>
+    <t>SSSOM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,19 +653,28 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF1F2328"/>
-      <name val="Segoe UI"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,12 +699,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -666,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -677,16 +723,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,17 +1077,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="121.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1083,7 +1139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1218,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1245,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1215,7 +1271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1319,14 +1375,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1345,14 +1401,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1371,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +1453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1423,14 +1479,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1449,7 +1505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1475,14 +1531,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1501,7 +1557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1527,7 +1583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1631,7 +1687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +1739,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1723,18 +1779,18 @@
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="6" width="40.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="6" width="40.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
@@ -1760,7 +1816,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1778,7 +1834,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1796,7 +1852,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1814,7 +1870,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -1835,7 +1891,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -1853,7 +1909,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -1871,7 +1927,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1889,7 +1945,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -1907,7 +1963,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1925,7 +1981,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -1943,7 +1999,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -1961,7 +2017,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -1979,7 +2035,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -1997,7 +2053,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -2015,7 +2071,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -2033,7 +2089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -2041,7 +2097,7 @@
         <v>43</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F17" t="s">
@@ -2054,7 +2110,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2128,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2090,7 +2146,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2108,7 +2164,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -2126,7 +2182,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -2144,7 +2200,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2162,7 +2218,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2180,7 +2236,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2198,7 +2254,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2216,7 +2272,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -2233,7 +2289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2250,7 +2306,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2267,7 +2323,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -2287,7 +2343,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E33" s="3" t="s">
         <v>26</v>
       </c>
@@ -2313,57 +2369,57 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="104.140625" customWidth="1"/>
+    <col min="1" max="1" width="104.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -2375,81 +2431,81 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O1" s="12"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -2464,13 +2520,13 @@
       <c r="F2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H2" t="s">
         <v>106</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="11">
         <v>45292</v>
       </c>
       <c r="K2" t="s">
@@ -2486,11 +2542,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
@@ -2505,13 +2561,13 @@
       <c r="F3" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H3" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="11">
         <v>45292</v>
       </c>
       <c r="K3" t="s">
@@ -2527,11 +2583,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -2546,13 +2602,13 @@
       <c r="F4" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H4" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="11">
         <v>45292</v>
       </c>
       <c r="K4" t="s">
@@ -2568,11 +2624,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
@@ -2587,13 +2643,13 @@
       <c r="F5" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H5" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="11">
         <v>45292</v>
       </c>
       <c r="K5" t="s">
@@ -2609,11 +2665,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" t="s">
         <v>146</v>
       </c>
       <c r="C6" t="s">
@@ -2628,13 +2684,13 @@
       <c r="F6" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="11">
         <v>45292</v>
       </c>
       <c r="K6" t="s">
@@ -2650,11 +2706,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" t="s">
         <v>148</v>
       </c>
       <c r="C7" t="s">
@@ -2669,13 +2725,13 @@
       <c r="F7" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H7" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="11">
         <v>45292</v>
       </c>
       <c r="K7" t="s">
@@ -2691,11 +2747,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" t="s">
         <v>149</v>
       </c>
       <c r="C8" t="s">
@@ -2710,13 +2766,13 @@
       <c r="F8" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H8" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="11">
         <v>45292</v>
       </c>
       <c r="K8" t="s">
@@ -2732,11 +2788,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" t="s">
         <v>150</v>
       </c>
       <c r="C9" t="s">
@@ -2751,13 +2807,13 @@
       <c r="F9" t="s">
         <v>94</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H9" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="11">
         <v>45292</v>
       </c>
       <c r="K9" t="s">
@@ -2773,11 +2829,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
@@ -2792,13 +2848,13 @@
       <c r="F10" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H10" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="11">
         <v>45292</v>
       </c>
       <c r="K10" t="s">
@@ -2814,11 +2870,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11" t="s">
@@ -2833,13 +2889,13 @@
       <c r="F11" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H11" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="11">
         <v>45292</v>
       </c>
       <c r="K11" t="s">
@@ -2855,11 +2911,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" t="s">
         <v>153</v>
       </c>
       <c r="C12" t="s">
@@ -2874,13 +2930,13 @@
       <c r="F12" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H12" t="s">
         <v>106</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="11">
         <v>45292</v>
       </c>
       <c r="K12" t="s">
@@ -2896,11 +2952,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
@@ -2915,13 +2971,13 @@
       <c r="F13" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H13" t="s">
         <v>106</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="11">
         <v>45292</v>
       </c>
       <c r="K13" t="s">
@@ -2937,12 +2993,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>40</v>
+        <v>141</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>95</v>
@@ -2956,34 +3012,25 @@
       <c r="F14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>105</v>
+      <c r="G14" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="H14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I14" s="9">
-        <v>45292</v>
+        <v>165</v>
+      </c>
+      <c r="I14" s="11">
+        <v>45413</v>
       </c>
       <c r="K14" t="s">
-        <v>108</v>
-      </c>
-      <c r="L14" t="s">
-        <v>103</v>
-      </c>
-      <c r="M14" t="s">
-        <v>109</v>
-      </c>
-      <c r="N14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>159</v>
+        <v>143</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>95</v>
@@ -2997,13 +3044,13 @@
       <c r="F15" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H15" t="s">
         <v>106</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="11">
         <v>45292</v>
       </c>
       <c r="K15" t="s">
@@ -3019,32 +3066,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>43</v>
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H16" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="11">
         <v>45292</v>
       </c>
       <c r="K16" t="s">
@@ -3060,32 +3107,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H17" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="11">
         <v>45292</v>
       </c>
       <c r="K17" t="s">
@@ -3101,32 +3148,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" t="s">
         <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H18" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="11">
         <v>45292</v>
       </c>
       <c r="K18" t="s">
@@ -3142,32 +3189,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>50</v>
+        <v>140</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H19" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="11">
         <v>45292</v>
       </c>
       <c r="K19" t="s">
@@ -3183,12 +3230,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>48</v>
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>95</v>
@@ -3202,13 +3249,13 @@
       <c r="F20" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H20" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="11">
         <v>45292</v>
       </c>
       <c r="K20" t="s">
@@ -3224,12 +3271,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
       </c>
       <c r="C21" t="s">
         <v>95</v>
@@ -3243,13 +3290,13 @@
       <c r="F21" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H21" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="11">
         <v>45292</v>
       </c>
       <c r="K21" t="s">
@@ -3265,12 +3312,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>158</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>157</v>
+        <v>143</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
       </c>
       <c r="C22" t="s">
         <v>95</v>
@@ -3284,13 +3331,13 @@
       <c r="F22" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H22" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="11">
         <v>45292</v>
       </c>
       <c r="K22" t="s">
@@ -3306,32 +3353,32 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>54</v>
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>157</v>
       </c>
       <c r="C23" t="s">
         <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H23" t="s">
         <v>106</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="11">
         <v>45292</v>
       </c>
       <c r="K23" t="s">
@@ -3347,12 +3394,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>155</v>
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>95</v>
@@ -3366,13 +3413,13 @@
       <c r="F24" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="14" t="s">
         <v>105</v>
       </c>
       <c r="H24" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="11">
         <v>45292</v>
       </c>
       <c r="K24" t="s">
@@ -3386,6 +3433,79 @@
       </c>
       <c r="N24" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="11">
+        <v>45292</v>
+      </c>
+      <c r="K25" t="s">
+        <v>108</v>
+      </c>
+      <c r="L25" t="s">
+        <v>103</v>
+      </c>
+      <c r="M25" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="11">
+        <v>45413</v>
+      </c>
+      <c r="K26" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3394,7 +3514,104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF210F61-45B4-45D2-ACBA-04A2FFFF0FEF}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5546875" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16">
+        <v>45436</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -3670,7 +3887,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
@@ -3687,7 +3904,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3696,57 +3913,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3765,7 +3940,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3776,18 +3951,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
NESP-GET converted to RDF/TTL
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Marine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732BF563-AF75-47D0-87BD-B9C3D16DF77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038C2624-E27A-4FC3-A5D8-397B161BC03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="720" windowWidth="19425" windowHeight="15345" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="990" yWindow="3480" windowWidth="34665" windowHeight="10815" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk_V1" sheetId="1" r:id="rId1"/>
@@ -2401,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD19"/>
     </sheetView>
   </sheetViews>
@@ -2459,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,8 +2570,8 @@
         <v>104</v>
       </c>
       <c r="O2" s="20" t="str">
-        <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET")</f>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET</v>
+        <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET - ", ROW(B2)-1)</f>
+        <v>Shelf unvegetated sediments - mapping to IUCN GET - 1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2615,8 +2615,8 @@
         <v>104</v>
       </c>
       <c r="O3" s="20" t="str">
-        <f t="shared" ref="O3:O25" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET")</f>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET</v>
+        <f t="shared" ref="O3:O26" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1)</f>
+        <v>Shelf unvegetated sediments - mapping to IUCN GET - 2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="O4" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET</v>
+        <v>Shelf unvegetated sediments - mapping to IUCN GET - 3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="O5" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET</v>
+        <v>Shelf unvegetated sediments - mapping to IUCN GET - 4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="O6" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Upper slope unvegetated sediments - mapping to IUCN GET</v>
+        <v>Upper slope unvegetated sediments - mapping to IUCN GET - 5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="O7" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Mid slope sediments - mapping to IUCN GET</v>
+        <v>Mid slope sediments - mapping to IUCN GET - 6</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="O8" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Lower slope reef and soft sediments - mapping to IUCN GET</v>
+        <v>Lower slope reef and soft sediments - mapping to IUCN GET - 7</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="O9" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Abyssal reef and sediments - mapping to IUCN GET</v>
+        <v>Abyssal reef and sediments - mapping to IUCN GET - 8</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2931,7 +2931,7 @@
       </c>
       <c r="O10" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Seamount sediments - mapping to IUCN GET</v>
+        <v>Seamount sediments - mapping to IUCN GET - 9</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
       </c>
       <c r="O11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Seamount reefs - mapping to IUCN GET</v>
+        <v>Seamount reefs - mapping to IUCN GET - 10</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="O12" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shelf incised canyons - mapping to IUCN GET</v>
+        <v>Shelf incised canyons - mapping to IUCN GET - 11</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="O13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shelf vegetated sediments - mapping to IUCN GET</v>
+        <v>Shelf vegetated sediments - mapping to IUCN GET - 12</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="O14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Mesophotic coral reefs - mapping to IUCN GET</v>
+        <v>Mesophotic coral reefs - mapping to IUCN GET - 13</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3147,7 +3147,7 @@
       </c>
       <c r="O15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Oceanic shallow coral reefs - mapping to IUCN GET</v>
+        <v>Oceanic shallow coral reefs - mapping to IUCN GET - 14</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
       </c>
       <c r="O16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shallow coral reefs - mapping to IUCN GET</v>
+        <v>Shallow coral reefs - mapping to IUCN GET - 15</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="O17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET</v>
+        <v>Shallow rocky reefs - mapping to IUCN GET - 16</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="O18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET</v>
+        <v>Shallow rocky reefs - mapping to IUCN GET - 17</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="O19" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET</v>
+        <v>Shallow rocky reefs - mapping to IUCN GET - 18</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="O20" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET</v>
+        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET - 19</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="O21" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Mesophotic rocky reefs - mapping to IUCN GET</v>
+        <v>Mesophotic rocky reefs - mapping to IUCN GET - 20</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="O22" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET</v>
+        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET - 21</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="O23" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Rariophotic shelf reefs - mapping to IUCN GET</v>
+        <v>Rariophotic shelf reefs - mapping to IUCN GET - 22</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="O24" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Upper slope reefs - mapping to IUCN GET</v>
+        <v>Upper slope reefs - mapping to IUCN GET - 23</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="O25" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Mid slope reef - mapping to IUCN GET</v>
+        <v>Mid slope reef - mapping to IUCN GET - 24</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3630,6 +3630,10 @@
       </c>
       <c r="K26" t="s">
         <v>149</v>
+      </c>
+      <c r="O26" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Islands (including cays and islets) - mapping to IUCN GET - 25</v>
       </c>
     </row>
   </sheetData>
@@ -3686,6 +3690,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -3961,33 +3982,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -4037,7 +4032,27 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4056,29 +4071,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Marine_IUCN crosswalk to fix order of narrow matches.
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Marine-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Marine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038C2624-E27A-4FC3-A5D8-397B161BC03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8179DDB0-47BB-47E8-9109-18956A013A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="3480" windowWidth="34665" windowHeight="10815" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="Crosswalk_V1" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,12 @@
     <sheet name="header" sheetId="5" r:id="rId3"/>
     <sheet name="SSSOM" sheetId="4" r:id="rId4"/>
     <sheet name="CHANGE_LOG" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -47,10 +37,19 @@
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{61E97ACF-2248-410F-BA66-E912F5FD73E7}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Is this actually the mapping author? </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="181">
   <si>
     <t>Realm</t>
   </si>
@@ -611,6 +610,12 @@
   </si>
   <si>
     <t>map: http://w3id.org/env/neap/nesp-get/</t>
+  </si>
+  <si>
+    <t>CKM</t>
+  </si>
+  <si>
+    <t>Changed order of narrow matches.</t>
   </si>
 </sst>
 </file>
@@ -803,9 +808,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -843,7 +848,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -949,7 +954,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1091,7 +1096,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2459,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,9 +2574,9 @@
       <c r="N2" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="20" t="str">
-        <f>_xlfn.CONCAT(B2, " - mapping to IUCN GET - ", ROW(B2)-1)</f>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET - 1</v>
+      <c r="O2" s="20" t="e">
+        <f ca="1">_xlfn.CONCAT(B2, " - mapping to IUCN GET - ", ROW(B2)-1)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2614,9 +2619,9 @@
       <c r="N3" t="s">
         <v>104</v>
       </c>
-      <c r="O3" s="20" t="str">
-        <f t="shared" ref="O3:O26" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1)</f>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET - 2</v>
+      <c r="O3" s="20" t="e">
+        <f t="shared" ref="O3:O26" ca="1" si="0">_xlfn.CONCAT(B3, " - mapping to IUCN GET - ", ROW(B3)-1)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2659,9 +2664,9 @@
       <c r="N4" t="s">
         <v>104</v>
       </c>
-      <c r="O4" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET - 3</v>
+      <c r="O4" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2704,9 +2709,9 @@
       <c r="N5" t="s">
         <v>104</v>
       </c>
-      <c r="O5" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shelf unvegetated sediments - mapping to IUCN GET - 4</v>
+      <c r="O5" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2749,9 +2754,9 @@
       <c r="N6" t="s">
         <v>104</v>
       </c>
-      <c r="O6" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Upper slope unvegetated sediments - mapping to IUCN GET - 5</v>
+      <c r="O6" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2794,9 +2799,9 @@
       <c r="N7" t="s">
         <v>104</v>
       </c>
-      <c r="O7" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Mid slope sediments - mapping to IUCN GET - 6</v>
+      <c r="O7" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2839,9 +2844,9 @@
       <c r="N8" t="s">
         <v>104</v>
       </c>
-      <c r="O8" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Lower slope reef and soft sediments - mapping to IUCN GET - 7</v>
+      <c r="O8" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2884,9 +2889,9 @@
       <c r="N9" t="s">
         <v>104</v>
       </c>
-      <c r="O9" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Abyssal reef and sediments - mapping to IUCN GET - 8</v>
+      <c r="O9" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2929,9 +2934,9 @@
       <c r="N10" t="s">
         <v>104</v>
       </c>
-      <c r="O10" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Seamount sediments - mapping to IUCN GET - 9</v>
+      <c r="O10" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2974,9 +2979,9 @@
       <c r="N11" t="s">
         <v>104</v>
       </c>
-      <c r="O11" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Seamount reefs - mapping to IUCN GET - 10</v>
+      <c r="O11" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3019,9 +3024,9 @@
       <c r="N12" t="s">
         <v>104</v>
       </c>
-      <c r="O12" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shelf incised canyons - mapping to IUCN GET - 11</v>
+      <c r="O12" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3064,9 +3069,9 @@
       <c r="N13" t="s">
         <v>104</v>
       </c>
-      <c r="O13" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shelf vegetated sediments - mapping to IUCN GET - 12</v>
+      <c r="O13" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3100,9 +3105,9 @@
       <c r="K14" t="s">
         <v>149</v>
       </c>
-      <c r="O14" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Mesophotic coral reefs - mapping to IUCN GET - 13</v>
+      <c r="O14" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3145,9 +3150,9 @@
       <c r="N15" t="s">
         <v>104</v>
       </c>
-      <c r="O15" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Oceanic shallow coral reefs - mapping to IUCN GET - 14</v>
+      <c r="O15" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3190,9 +3195,9 @@
       <c r="N16" t="s">
         <v>104</v>
       </c>
-      <c r="O16" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shallow coral reefs - mapping to IUCN GET - 15</v>
+      <c r="O16" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3206,10 +3211,10 @@
         <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
         <v>89</v>
@@ -3235,9 +3240,9 @@
       <c r="N17" t="s">
         <v>104</v>
       </c>
-      <c r="O17" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET - 16</v>
+      <c r="O17" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3280,9 +3285,9 @@
       <c r="N18" t="s">
         <v>104</v>
       </c>
-      <c r="O18" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET - 17</v>
+      <c r="O18" s="20" t="e">
+        <f ca="1">_xlfn.CONCAT(B18, " - mapping to IUCN GET - ", ROW(B18)-1)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3296,10 +3301,10 @@
         <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
         <v>89</v>
@@ -3325,9 +3330,9 @@
       <c r="N19" t="s">
         <v>104</v>
       </c>
-      <c r="O19" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Shallow rocky reefs - mapping to IUCN GET - 18</v>
+      <c r="O19" s="20" t="e">
+        <f ca="1">_xlfn.CONCAT(B19, " - mapping to IUCN GET - ", ROW(B19)-1)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -3370,9 +3375,9 @@
       <c r="N20" t="s">
         <v>104</v>
       </c>
-      <c r="O20" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET - 19</v>
+      <c r="O20" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -3415,9 +3420,9 @@
       <c r="N21" t="s">
         <v>104</v>
       </c>
-      <c r="O21" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Mesophotic rocky reefs - mapping to IUCN GET - 20</v>
+      <c r="O21" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3460,9 +3465,9 @@
       <c r="N22" t="s">
         <v>104</v>
       </c>
-      <c r="O22" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Oceanic mesophotic coral reefs - mapping to IUCN GET - 21</v>
+      <c r="O22" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3505,9 +3510,9 @@
       <c r="N23" t="s">
         <v>104</v>
       </c>
-      <c r="O23" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Rariophotic shelf reefs - mapping to IUCN GET - 22</v>
+      <c r="O23" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3550,9 +3555,9 @@
       <c r="N24" t="s">
         <v>104</v>
       </c>
-      <c r="O24" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Upper slope reefs - mapping to IUCN GET - 23</v>
+      <c r="O24" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3595,9 +3600,9 @@
       <c r="N25" t="s">
         <v>104</v>
       </c>
-      <c r="O25" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Mid slope reef - mapping to IUCN GET - 24</v>
+      <c r="O25" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3631,9 +3636,9 @@
       <c r="K26" t="s">
         <v>149</v>
       </c>
-      <c r="O26" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Islands (including cays and islets) - mapping to IUCN GET - 25</v>
+      <c r="O26" s="20" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -3644,7 +3649,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF210F61-45B4-45D2-ACBA-04A2FFFF0FEF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -3684,29 +3689,112 @@
         <v>156</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>45498</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF3C425-A9ED-4090-870D-14240F6A5903}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -3982,7 +4070,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -4032,27 +4146,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4071,18 +4165,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed narrow match for M1.7
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine-IUCNGET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Marine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E601F8-7715-4E75-87E2-AF10D44E37CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1B2800-F0A6-4397-A87E-5DD80E81022B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
@@ -2465,7 +2465,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,10 +2590,10 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
         <v>89</v>
@@ -2635,10 +2635,10 @@
         <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
         <v>89</v>
@@ -2680,10 +2680,10 @@
         <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>89</v>
@@ -2710,7 +2710,7 @@
         <v>104</v>
       </c>
       <c r="O5" s="20" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">_xlfn.CONCAT(B5, " - mapping to IUCN GET - ", ROW(B5)-1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -3795,6 +3795,82 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -4070,83 +4146,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4163,31 +4190,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>